<commit_message>
IA-3793 validate xlsform handle or_other and spaces more robustly
</commit_message>
<xml_diff>
--- a/iaso/tests/fixtures/odk_invalid_xlsform.xlsx
+++ b/iaso/tests/fixtures/odk_invalid_xlsform.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="155">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -488,6 +488,40 @@
     <t xml:space="preserve">${test_unknown_ref}</t>
   </si>
   <si>
+    <t xml:space="preserve">select_one ration_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ration_type_tsfp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose ration type. Suggested rations type: RUSF 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">select_one  ration_type </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">or_other</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ration_type_with_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose ration type. Suggested rations type: RUSF 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">list_name</t>
   </si>
   <si>
@@ -522,6 +556,21 @@
   </si>
   <si>
     <t xml:space="preserve">buffalo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ration_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rutf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rusf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUSF</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -546,10 +595,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -628,17 +678,48 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="WenQuanYi Micro Hei"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -675,7 +756,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -748,8 +829,32 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -761,6 +866,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFF2CC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -875,10 +1040,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O100"/>
+  <dimension ref="A1:O103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A75" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C103" activeCellId="0" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2235,6 +2400,30 @@
       <c r="N100" s="17"/>
       <c r="O100" s="17"/>
     </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B102" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D102" s="19"/>
+      <c r="E102" s="20"/>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2251,12 +2440,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.23828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2267,7 +2456,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -2281,67 +2470,89 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="18"/>
+        <v>134</v>
+      </c>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E3" s="18"/>
+        <v>135</v>
+      </c>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C7" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>148</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2376,27 +2587,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix typo in xlsform
</commit_message>
<xml_diff>
--- a/iaso/tests/fixtures/odk_invalid_xlsform.xlsx
+++ b/iaso/tests/fixtures/odk_invalid_xlsform.xlsx
@@ -425,7 +425,7 @@
     <t xml:space="preserve">This should throw a warning a_text_without_a_name</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one doenst_exist</t>
+    <t xml:space="preserve">select_one doesnt_exist</t>
   </si>
   <si>
     <t xml:space="preserve">nonexistingchoices</t>
@@ -503,6 +503,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">select_one  ration_type </t>
     </r>
@@ -511,6 +512,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">or_other</t>
     </r>
@@ -599,7 +601,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -692,14 +694,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -829,31 +826,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1042,8 +1039,8 @@
   </sheetPr>
   <dimension ref="A1:O103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A75" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C103" activeCellId="0" sqref="C103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2445,7 +2442,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="bottomLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.23828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix test for it
</commit_message>
<xml_diff>
--- a/iaso/tests/fixtures/odk_invalid_xlsform.xlsx
+++ b/iaso/tests/fixtures/odk_invalid_xlsform.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beygorghor/WORK/BLSQ/iaso/iaso/iaso/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1DFF59-0706-224E-99D4-37AD3A32AE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB2E17E-5F9B-6146-9F43-42959B7A97FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="-7060" windowWidth="68800" windowHeight="26480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-62180" yWindow="-6460" windowWidth="58640" windowHeight="22020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="13"/>
@@ -1176,49 +1176,45 @@
     </row>
     <row r="10" spans="1:12" ht="16">
       <c r="A10" s="8" t="s">
-        <v>155</v>
+        <v>21</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>157</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="9"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="K10" s="9"/>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" ht="16">
+    </row>
+    <row r="11" spans="1:12" ht="16.5" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="8"/>
+        <v>34</v>
+      </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K11" s="9"/>
+      <c r="J11" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="16.5" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D12" s="8"/>
       <c r="F12" s="1"/>
@@ -1226,35 +1222,32 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="16.5" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="D13" s="8"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>40</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1263,11 +1256,15 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="D15" s="8"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1276,267 +1273,257 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="K16" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="16.5" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="D17" s="11"/>
       <c r="E17" s="4"/>
-      <c r="K17" t="s">
-        <v>44</v>
-      </c>
-      <c r="L17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="16.5" customHeight="1">
+      <c r="J17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="16.5" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D18" s="11"/>
       <c r="E18" s="4"/>
       <c r="J18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="16.5" customHeight="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="11"/>
       <c r="E19" s="4"/>
-      <c r="J19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="16.5" customHeight="1">
+      <c r="K19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16.5" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="11"/>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
       <c r="E20" s="4"/>
-      <c r="K20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A21" s="4" t="s">
+      <c r="I20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="I21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="B21" t="s">
         <v>55</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="16.5" customHeight="1">
+    <row r="22" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="16.5" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="16.5" customHeight="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="28.5" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="28.5" customHeight="1">
+        <v>62</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="16.5" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="16.5" customHeight="1">
+        <v>64</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="16.5" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" t="s">
         <v>64</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="16.5" customHeight="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="16.5" customHeight="1">
       <c r="A27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="J27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="12" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="28.5" customHeight="1">
+      <c r="A30" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="11"/>
-      <c r="D27" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A28" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="J28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="12" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A29" s="4" t="s">
+      <c r="B30" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A31" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="16.5" customHeight="1">
+      <c r="A32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="12" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A33" t="s">
         <v>12</v>
       </c>
-      <c r="B29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="1" t="s">
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A33" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" t="s">
-        <v>79</v>
-      </c>
-    </row>
     <row r="34" spans="1:5" s="12" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" t="s">
-        <v>81</v>
-      </c>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
       <c r="D34"/>
-      <c r="E34" t="s">
-        <v>73</v>
-      </c>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" s="12" customFormat="1" ht="16.5" customHeight="1">
       <c r="A35" s="4"/>
@@ -1545,80 +1532,85 @@
       <c r="D35"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" s="12" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36"/>
-      <c r="E36" s="4"/>
+    <row r="36" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="16.5" customHeight="1">
       <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A39" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" t="s">
-        <v>84</v>
-      </c>
-      <c r="D39" t="s">
+    <row r="40" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A40" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A40" t="s">
+      <c r="E40" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A42" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A41" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" ht="16.5" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>23</v>
+        <v>88</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16.5" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" t="s">
@@ -1627,10 +1619,10 @@
     </row>
     <row r="45" spans="1:5" ht="16.5" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" t="s">
@@ -1639,10 +1631,10 @@
     </row>
     <row r="46" spans="1:5" ht="16.5" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" t="s">
@@ -1651,10 +1643,10 @@
     </row>
     <row r="47" spans="1:5" ht="16.5" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" t="s">
@@ -1663,10 +1655,10 @@
     </row>
     <row r="48" spans="1:5" ht="16.5" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" t="s">
@@ -1675,10 +1667,10 @@
     </row>
     <row r="49" spans="1:5" ht="16.5" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" t="s">
@@ -1687,10 +1679,10 @@
     </row>
     <row r="50" spans="1:5" ht="16.5" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" t="s">
@@ -1699,10 +1691,10 @@
     </row>
     <row r="51" spans="1:5" ht="16.5" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" t="s">
@@ -1710,51 +1702,50 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>101</v>
-      </c>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
       <c r="C52" s="4"/>
-      <c r="D52" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="53" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
+      <c r="A53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="16.5" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>102</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B54" s="4"/>
       <c r="C54" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="16.5" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" s="4"/>
+        <v>105</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="C55" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="16.5" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="16.5" customHeight="1">
@@ -1764,112 +1755,118 @@
       <c r="B57" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>109</v>
-      </c>
+      <c r="C57" s="4"/>
     </row>
     <row r="58" spans="1:5" ht="16.5" customHeight="1">
       <c r="A58" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C58" s="4"/>
+        <v>110</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="16.5" customHeight="1">
       <c r="A59" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A60" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>112</v>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="E60" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="E61" t="s">
-        <v>113</v>
+      <c r="A61" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A62" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>114</v>
-      </c>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
     </row>
     <row r="63" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
+      <c r="A63" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A64" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>115</v>
-      </c>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
     </row>
     <row r="65" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
+      <c r="A65" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="66" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A66" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>116</v>
-      </c>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
     </row>
     <row r="67" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
+      <c r="A67" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="68" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A68" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>117</v>
-      </c>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
     </row>
     <row r="69" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-    </row>
-    <row r="70" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A70" s="4" t="s">
+      <c r="A69" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="B69" s="11" t="s">
         <v>118</v>
       </c>
+    </row>
+    <row r="71" spans="1:15" ht="16">
+      <c r="A71" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C71" s="4"/>
+      <c r="D71" t="s">
+        <v>3</v>
+      </c>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="14"/>
+      <c r="N71" s="14"/>
+      <c r="O71" s="14"/>
     </row>
     <row r="72" spans="1:15" ht="16">
       <c r="A72" s="4" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" t="s">
@@ -1883,10 +1880,10 @@
     </row>
     <row r="73" spans="1:15" ht="16">
       <c r="A73" s="4" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" t="s">
@@ -1900,10 +1897,10 @@
     </row>
     <row r="74" spans="1:15" ht="16">
       <c r="A74" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" t="s">
@@ -1917,10 +1914,10 @@
     </row>
     <row r="75" spans="1:15" ht="16">
       <c r="A75" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" t="s">
@@ -1934,10 +1931,10 @@
     </row>
     <row r="76" spans="1:15" ht="16">
       <c r="A76" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" t="s">
@@ -1951,10 +1948,10 @@
     </row>
     <row r="77" spans="1:15" ht="16">
       <c r="A77" s="4" t="s">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" t="s">
@@ -1968,10 +1965,10 @@
     </row>
     <row r="78" spans="1:15" ht="16">
       <c r="A78" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" t="s">
@@ -1985,10 +1982,10 @@
     </row>
     <row r="79" spans="1:15" ht="16">
       <c r="A79" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" t="s">
@@ -2001,16 +1998,9 @@
       <c r="O79" s="14"/>
     </row>
     <row r="80" spans="1:15" ht="16">
-      <c r="A80" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>101</v>
-      </c>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
       <c r="C80" s="4"/>
-      <c r="D80" t="s">
-        <v>3</v>
-      </c>
       <c r="K80" s="13"/>
       <c r="L80" s="13"/>
       <c r="M80" s="14"/>
@@ -2018,9 +2008,18 @@
       <c r="O80" s="14"/>
     </row>
     <row r="81" spans="1:15" ht="16">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
+      <c r="A81" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>119</v>
+      </c>
       <c r="K81" s="13"/>
       <c r="L81" s="13"/>
       <c r="M81" s="14"/>
@@ -2029,16 +2028,13 @@
     </row>
     <row r="82" spans="1:15" ht="16">
       <c r="A82" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="I82" s="13" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="K82" s="13"/>
       <c r="L82" s="13"/>
@@ -2048,13 +2044,13 @@
     </row>
     <row r="83" spans="1:15" ht="16">
       <c r="A83" s="4" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="K83" s="13"/>
       <c r="L83" s="13"/>
@@ -2064,13 +2060,13 @@
     </row>
     <row r="84" spans="1:15" ht="16">
       <c r="A84" s="4" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K84" s="13"/>
       <c r="L84" s="13"/>
@@ -2085,9 +2081,7 @@
       <c r="B85" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>109</v>
-      </c>
+      <c r="C85" s="4"/>
       <c r="K85" s="13"/>
       <c r="L85" s="13"/>
       <c r="M85" s="14"/>
@@ -2099,9 +2093,11 @@
         <v>14</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C86" s="4"/>
+        <v>121</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="K86" s="13"/>
       <c r="L86" s="13"/>
       <c r="M86" s="14"/>
@@ -2110,13 +2106,10 @@
     </row>
     <row r="87" spans="1:15" ht="16">
       <c r="A87" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="K87" s="13"/>
       <c r="L87" s="13"/>
@@ -2125,12 +2118,9 @@
       <c r="O87" s="14"/>
     </row>
     <row r="88" spans="1:15" ht="16">
-      <c r="A88" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>112</v>
-      </c>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
       <c r="K88" s="13"/>
       <c r="L88" s="13"/>
       <c r="M88" s="14"/>
@@ -2138,9 +2128,12 @@
       <c r="O88" s="14"/>
     </row>
     <row r="89" spans="1:15" ht="16">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
+      <c r="A89" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>114</v>
+      </c>
       <c r="K89" s="13"/>
       <c r="L89" s="13"/>
       <c r="M89" s="14"/>
@@ -2148,12 +2141,9 @@
       <c r="O89" s="14"/>
     </row>
     <row r="90" spans="1:15" ht="16">
-      <c r="A90" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B90" s="11" t="s">
-        <v>114</v>
-      </c>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
       <c r="K90" s="13"/>
       <c r="L90" s="13"/>
       <c r="M90" s="14"/>
@@ -2161,9 +2151,12 @@
       <c r="O90" s="14"/>
     </row>
     <row r="91" spans="1:15" ht="16">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
+      <c r="A91" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>115</v>
+      </c>
       <c r="K91" s="13"/>
       <c r="L91" s="13"/>
       <c r="M91" s="14"/>
@@ -2171,12 +2164,9 @@
       <c r="O91" s="14"/>
     </row>
     <row r="92" spans="1:15" ht="16">
-      <c r="A92" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B92" s="11" t="s">
-        <v>115</v>
-      </c>
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
       <c r="K92" s="13"/>
       <c r="L92" s="13"/>
       <c r="M92" s="14"/>
@@ -2184,9 +2174,12 @@
       <c r="O92" s="14"/>
     </row>
     <row r="93" spans="1:15" ht="16">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
+      <c r="A93" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="K93" s="13"/>
       <c r="L93" s="13"/>
       <c r="M93" s="14"/>
@@ -2194,12 +2187,9 @@
       <c r="O93" s="14"/>
     </row>
     <row r="94" spans="1:15" ht="16">
-      <c r="A94" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>116</v>
-      </c>
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
       <c r="K94" s="13"/>
       <c r="L94" s="13"/>
       <c r="M94" s="14"/>
@@ -2207,9 +2197,12 @@
       <c r="O94" s="14"/>
     </row>
     <row r="95" spans="1:15" ht="16">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
+      <c r="A95" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>117</v>
+      </c>
       <c r="K95" s="13"/>
       <c r="L95" s="13"/>
       <c r="M95" s="14"/>
@@ -2217,12 +2210,9 @@
       <c r="O95" s="14"/>
     </row>
     <row r="96" spans="1:15" ht="16">
-      <c r="A96" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B96" s="11" t="s">
-        <v>117</v>
-      </c>
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
       <c r="K96" s="13"/>
       <c r="L96" s="13"/>
       <c r="M96" s="14"/>
@@ -2230,9 +2220,12 @@
       <c r="O96" s="14"/>
     </row>
     <row r="97" spans="1:15" ht="16">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
+      <c r="A97" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B97" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="K97" s="13"/>
       <c r="L97" s="13"/>
       <c r="M97" s="14"/>
@@ -2240,12 +2233,6 @@
       <c r="O97" s="14"/>
     </row>
     <row r="98" spans="1:15" ht="16">
-      <c r="A98" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B98" s="11" t="s">
-        <v>118</v>
-      </c>
       <c r="K98" s="13"/>
       <c r="L98" s="13"/>
       <c r="M98" s="14"/>
@@ -2253,6 +2240,15 @@
       <c r="O98" s="14"/>
     </row>
     <row r="99" spans="1:15" ht="16">
+      <c r="A99" t="s">
+        <v>38</v>
+      </c>
+      <c r="B99" t="s">
+        <v>122</v>
+      </c>
+      <c r="C99" t="s">
+        <v>123</v>
+      </c>
       <c r="K99" s="13"/>
       <c r="L99" s="13"/>
       <c r="M99" s="14"/>
@@ -2261,13 +2257,13 @@
     </row>
     <row r="100" spans="1:15" ht="16">
       <c r="A100" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B100" t="s">
-        <v>122</v>
-      </c>
-      <c r="C100" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="I100" t="s">
+        <v>125</v>
       </c>
       <c r="K100" s="13"/>
       <c r="L100" s="13"/>
@@ -2275,44 +2271,39 @@
       <c r="N100" s="14"/>
       <c r="O100" s="14"/>
     </row>
-    <row r="101" spans="1:15" ht="16">
-      <c r="A101" t="s">
-        <v>21</v>
-      </c>
-      <c r="B101" t="s">
-        <v>124</v>
-      </c>
-      <c r="I101" t="s">
-        <v>125</v>
-      </c>
-      <c r="K101" s="13"/>
-      <c r="L101" s="13"/>
-      <c r="M101" s="14"/>
-      <c r="N101" s="14"/>
-      <c r="O101" s="14"/>
-    </row>
-    <row r="103" spans="1:15" ht="14">
-      <c r="A103" s="15" t="s">
+    <row r="102" spans="1:15" ht="14">
+      <c r="A102" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B103" s="16" t="s">
+      <c r="B102" s="16" t="s">
         <v>127</v>
       </c>
+      <c r="C102" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D102" s="16"/>
+      <c r="E102" s="17"/>
+    </row>
+    <row r="103" spans="1:15">
+      <c r="A103" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B103" t="s">
+        <v>130</v>
+      </c>
       <c r="C103" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D103" s="16"/>
-      <c r="E103" s="17"/>
+        <v>131</v>
+      </c>
     </row>
     <row r="104" spans="1:15">
-      <c r="A104" s="18" t="s">
-        <v>129</v>
+      <c r="A104" t="s">
+        <v>155</v>
       </c>
       <c r="B104" t="s">
-        <v>130</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>131</v>
+        <v>156</v>
+      </c>
+      <c r="C104" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>